<commit_message>
Add Remote Sensing Guest Editor
</commit_message>
<xml_diff>
--- a/data/service.xlsx
+++ b/data/service.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
   <si>
     <t xml:space="preserve">what</t>
   </si>
@@ -49,6 +49,15 @@
     <t xml:space="preserve">Toowoomba, Queensland, AUS</t>
   </si>
   <si>
+    <t xml:space="preserve">Guest Editor for Special Issue on Remote Sensing and Crop Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDPI Remote Sensing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global</t>
+  </si>
+  <si>
     <t xml:space="preserve">Member</t>
   </si>
   <si>
@@ -68,9 +77,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tropical Plant Pathology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Global</t>
   </si>
   <si>
     <t xml:space="preserve">Co-Founder and Co-Director</t>
@@ -267,10 +273,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -314,245 +320,259 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="4" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>